<commit_message>
Add systemd service for backend
</commit_message>
<xml_diff>
--- a/Wiring Diagram.xlsx
+++ b/Wiring Diagram.xlsx
@@ -1,31 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024\FuelTankAutomation-HandyTruckLineInc\FuelTankAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347E0E98-9286-4E7F-8EB3-561AFF37EF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slot 0" sheetId="1" r:id="rId1"/>
-    <sheet name="Slot 1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Slot 1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
   <si>
     <t>TB No</t>
   </si>
@@ -277,13 +290,70 @@
   </si>
   <si>
     <t>Val3-PIN1</t>
+  </si>
+  <si>
+    <t>C2-14D1</t>
+  </si>
+  <si>
+    <t>0V</t>
+  </si>
+  <si>
+    <t>+24V</t>
+  </si>
+  <si>
+    <t>Please refer to the Vavle PINs:</t>
+  </si>
+  <si>
+    <t>Valve1-NO4</t>
+  </si>
+  <si>
+    <t>Valve1-NO5</t>
+  </si>
+  <si>
+    <t>Valve2-NO4</t>
+  </si>
+  <si>
+    <t>Valve2-NO5</t>
+  </si>
+  <si>
+    <t>Valve3-NO4</t>
+  </si>
+  <si>
+    <t>Valve3-NO5</t>
+  </si>
+  <si>
+    <t>Valve1-NO2</t>
+  </si>
+  <si>
+    <t>Valve1-NO1</t>
+  </si>
+  <si>
+    <t>Valve2-NO2</t>
+  </si>
+  <si>
+    <t>Valve2-NO1</t>
+  </si>
+  <si>
+    <t>Valve3-NO2</t>
+  </si>
+  <si>
+    <t>Valve3-NO1</t>
+  </si>
+  <si>
+    <t>Vavle1-NO3</t>
+  </si>
+  <si>
+    <t>Valve2-NO3</t>
+  </si>
+  <si>
+    <t>Valve3-NO3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,8 +388,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,8 +446,35 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -386,14 +512,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,9 +587,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,10 +596,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="3" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="4" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
+    <cellStyle name="60% - Accent5" xfId="7" builtinId="48"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
@@ -2046,108 +2252,55 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>484094</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>82476</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>485767</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>52740</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>185949</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>176622</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Connector 1">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DBD477-DF42-4655-B5B3-536D41B73A96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E45AF83-8E64-4346-99C0-51F6E0DA3150}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5254214" y="2277036"/>
-          <a:ext cx="1673" cy="1250424"/>
+          <a:off x="3352800" y="809625"/>
+          <a:ext cx="3891174" cy="3900897"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="25400"/>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>974481</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>491528</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>110856</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655E15DD-303C-4CCC-8B6E-C03C1172E7A5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4088423" y="2388577"/>
-          <a:ext cx="1106990" cy="8279"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -3176,110 +3329,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>21981</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>117231</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>179294</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Straight Connector 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CBBF5ED-3829-4247-91A5-00FB9F8A7C58}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4117731" y="2593731"/>
-          <a:ext cx="3403140" cy="35169"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>176191</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>144884</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>181604</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>65478</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Straight Connector 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBD0C978-2BFE-4A9A-B84C-096A9C612EE6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="20" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7605691" y="2522324"/>
-          <a:ext cx="5413" cy="1017874"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>690283</xdr:colOff>
       <xdr:row>22</xdr:row>
@@ -3900,10 +3949,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E20"/>
     </sheetView>
   </sheetViews>
@@ -3939,7 +3988,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3954,7 +4003,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -3969,7 +4018,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -3984,7 +4033,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -3994,12 +4043,12 @@
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -4009,12 +4058,12 @@
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -4022,12 +4071,12 @@
         <v>37</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -4037,12 +4086,12 @@
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -4052,12 +4101,12 @@
       <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -4070,7 +4119,7 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -4083,7 +4132,7 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -4096,7 +4145,7 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3">
         <v>1</v>
       </c>
@@ -4106,12 +4155,12 @@
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3">
         <v>2</v>
       </c>
@@ -4126,7 +4175,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3">
         <v>3</v>
       </c>
@@ -4136,12 +4185,12 @@
       <c r="D15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3">
         <v>4</v>
       </c>
@@ -4151,12 +4200,12 @@
       <c r="D16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
@@ -4167,7 +4216,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="3">
         <v>5</v>
       </c>
@@ -4177,12 +4226,12 @@
       <c r="D18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="3">
         <v>6</v>
       </c>
@@ -4192,7 +4241,7 @@
       <c r="D19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H19" t="s">
@@ -4203,7 +4252,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
@@ -4211,7 +4260,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4259,11 +4308,247 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07F7AC3-853B-47B2-A4F6-6BAD3D73A01D}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="9.140625" style="16"/>
+    <col min="3" max="3" width="14.42578125" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="17">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="17">
+        <v>2</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="17">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="17">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="17">
+        <v>5</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="17">
+        <v>6</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="17">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="17">
+        <v>2</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="17">
+        <v>3</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="17">
+        <v>5</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="17">
+        <v>6</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4298,7 +4583,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -4313,7 +4598,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -4328,7 +4613,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -4343,7 +4628,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -4353,12 +4638,12 @@
       <c r="D5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -4368,12 +4653,12 @@
       <c r="D6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -4381,12 +4666,12 @@
         <v>37</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -4396,12 +4681,12 @@
       <c r="D8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -4411,12 +4696,12 @@
       <c r="D9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -4429,7 +4714,7 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -4442,7 +4727,7 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -4455,7 +4740,7 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3">
         <v>1</v>
       </c>
@@ -4465,12 +4750,12 @@
       <c r="D13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3">
         <v>2</v>
       </c>
@@ -4485,7 +4770,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3">
         <v>3</v>
       </c>
@@ -4495,12 +4780,12 @@
       <c r="D15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3">
         <v>4</v>
       </c>
@@ -4510,12 +4795,12 @@
       <c r="D16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
@@ -4526,7 +4811,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="3">
         <v>5</v>
       </c>
@@ -4536,12 +4821,12 @@
       <c r="D18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="3">
         <v>6</v>
       </c>
@@ -4551,7 +4836,7 @@
       <c r="D19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H19" t="s">
@@ -4562,7 +4847,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
@@ -4570,7 +4855,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>